<commit_message>
Support RGB888-image display on LCD.
</commit_message>
<xml_diff>
--- a/12.imx6ull/2.framebuffer/example.xlsx
+++ b/12.imx6ull/2.framebuffer/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375"/>
+    <workbookView windowWidth="22176" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,17 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.4"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -176,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +192,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.35"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -342,12 +391,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,138 +539,168 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -941,14 +1014,1224 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:BV23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="2.62037037037037" defaultRowHeight="14.15" customHeight="1"/>
+  <cols>
+    <col min="1" max="16384" width="2.62037037037037" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" spans="1:74">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="3"/>
+      <c r="BE1" s="3"/>
+      <c r="BF1" s="3"/>
+      <c r="BG1" s="3"/>
+      <c r="BH1" s="3"/>
+      <c r="BI1" s="3"/>
+      <c r="BJ1" s="3"/>
+      <c r="BK1" s="3"/>
+      <c r="BL1" s="3"/>
+      <c r="BM1" s="3"/>
+      <c r="BN1" s="4"/>
+      <c r="BO1" s="4"/>
+      <c r="BP1" s="4"/>
+      <c r="BQ1" s="4"/>
+      <c r="BR1" s="4"/>
+      <c r="BS1" s="4"/>
+      <c r="BT1" s="4"/>
+      <c r="BU1" s="4"/>
+      <c r="BV1" s="3"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:74">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="BC2" s="3"/>
+      <c r="BD2" s="3"/>
+      <c r="BE2" s="6"/>
+      <c r="BF2" s="6"/>
+      <c r="BG2" s="6"/>
+      <c r="BH2" s="6"/>
+      <c r="BI2" s="6"/>
+      <c r="BJ2" s="6"/>
+      <c r="BK2" s="6"/>
+      <c r="BL2" s="6"/>
+      <c r="BM2" s="6"/>
+      <c r="BN2" s="4"/>
+      <c r="BO2" s="4"/>
+      <c r="BP2" s="4"/>
+      <c r="BQ2" s="4"/>
+      <c r="BR2" s="4"/>
+      <c r="BS2" s="4"/>
+      <c r="BT2" s="4"/>
+      <c r="BU2" s="4"/>
+      <c r="BV2" s="3"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:74">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="BC3" s="3"/>
+      <c r="BD3" s="3"/>
+      <c r="BE3" s="6"/>
+      <c r="BF3" s="6"/>
+      <c r="BG3" s="6"/>
+      <c r="BH3" s="6"/>
+      <c r="BI3" s="6"/>
+      <c r="BJ3" s="6"/>
+      <c r="BK3" s="6"/>
+      <c r="BL3" s="6"/>
+      <c r="BM3" s="6"/>
+      <c r="BN3" s="4"/>
+      <c r="BO3" s="4"/>
+      <c r="BP3" s="4"/>
+      <c r="BQ3" s="4"/>
+      <c r="BR3" s="4"/>
+      <c r="BS3" s="4"/>
+      <c r="BT3" s="4"/>
+      <c r="BU3" s="4"/>
+      <c r="BV3" s="3"/>
+    </row>
+    <row r="4" customHeight="1" spans="1:74">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="BC4" s="3"/>
+      <c r="BD4" s="3"/>
+      <c r="BE4" s="6"/>
+      <c r="BF4" s="6"/>
+      <c r="BG4" s="6"/>
+      <c r="BH4" s="6"/>
+      <c r="BI4" s="6"/>
+      <c r="BJ4" s="6"/>
+      <c r="BK4" s="6"/>
+      <c r="BL4" s="6"/>
+      <c r="BM4" s="6"/>
+      <c r="BN4" s="4"/>
+      <c r="BO4" s="4"/>
+      <c r="BP4" s="4"/>
+      <c r="BQ4" s="4"/>
+      <c r="BR4" s="4"/>
+      <c r="BS4" s="4"/>
+      <c r="BT4" s="4"/>
+      <c r="BU4" s="4"/>
+      <c r="BV4" s="3"/>
+    </row>
+    <row r="5" customHeight="1" spans="1:74">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="BC5" s="5"/>
+      <c r="BD5" s="5"/>
+      <c r="BE5" s="5"/>
+      <c r="BF5" s="5"/>
+      <c r="BG5" s="5"/>
+      <c r="BH5" s="5"/>
+      <c r="BI5" s="6"/>
+      <c r="BJ5" s="6"/>
+      <c r="BK5" s="6"/>
+      <c r="BL5" s="6"/>
+      <c r="BM5" s="6"/>
+      <c r="BN5" s="4"/>
+      <c r="BO5" s="4"/>
+      <c r="BP5" s="4"/>
+      <c r="BQ5" s="4"/>
+      <c r="BR5" s="4"/>
+      <c r="BS5" s="4"/>
+      <c r="BT5" s="4"/>
+      <c r="BU5" s="4"/>
+      <c r="BV5" s="3"/>
+    </row>
+    <row r="6" customHeight="1" spans="1:74">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="BC6" s="5"/>
+      <c r="BD6" s="5"/>
+      <c r="BE6" s="5"/>
+      <c r="BF6" s="5"/>
+      <c r="BG6" s="5"/>
+      <c r="BH6" s="5"/>
+      <c r="BI6" s="7"/>
+      <c r="BJ6" s="7"/>
+      <c r="BK6" s="7"/>
+      <c r="BL6" s="7"/>
+      <c r="BM6" s="7"/>
+      <c r="BN6" s="7"/>
+      <c r="BO6" s="7"/>
+      <c r="BP6" s="9"/>
+      <c r="BQ6" s="9"/>
+      <c r="BR6" s="9"/>
+      <c r="BS6" s="3"/>
+      <c r="BT6" s="3"/>
+      <c r="BU6" s="3"/>
+      <c r="BV6" s="3"/>
+    </row>
+    <row r="7" customHeight="1" spans="1:74">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="BC7" s="5"/>
+      <c r="BD7" s="5"/>
+      <c r="BE7" s="5"/>
+      <c r="BF7" s="5"/>
+      <c r="BG7" s="5"/>
+      <c r="BH7" s="5"/>
+      <c r="BI7" s="7"/>
+      <c r="BJ7" s="7"/>
+      <c r="BK7" s="7"/>
+      <c r="BL7" s="8"/>
+      <c r="BM7" s="8"/>
+      <c r="BN7" s="8"/>
+      <c r="BO7" s="8"/>
+      <c r="BP7" s="8"/>
+      <c r="BQ7" s="8"/>
+      <c r="BR7" s="8"/>
+      <c r="BS7" s="10"/>
+      <c r="BT7" s="10"/>
+      <c r="BU7" s="10"/>
+      <c r="BV7" s="10"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:74">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="BC8" s="5"/>
+      <c r="BD8" s="5"/>
+      <c r="BE8" s="5"/>
+      <c r="BF8" s="5"/>
+      <c r="BG8" s="5"/>
+      <c r="BH8" s="5"/>
+      <c r="BI8" s="9"/>
+      <c r="BJ8" s="9"/>
+      <c r="BK8" s="9"/>
+      <c r="BL8" s="8"/>
+      <c r="BM8" s="8"/>
+      <c r="BN8" s="8"/>
+      <c r="BO8" s="8"/>
+      <c r="BP8" s="8"/>
+      <c r="BQ8" s="8"/>
+      <c r="BR8" s="8"/>
+      <c r="BS8" s="10"/>
+      <c r="BT8" s="10"/>
+      <c r="BU8" s="10"/>
+      <c r="BV8" s="10"/>
+    </row>
+    <row r="9" customHeight="1" spans="1:74">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="BC9" s="5"/>
+      <c r="BD9" s="5"/>
+      <c r="BE9" s="5"/>
+      <c r="BF9" s="5"/>
+      <c r="BG9" s="5"/>
+      <c r="BH9" s="5"/>
+      <c r="BI9" s="9"/>
+      <c r="BJ9" s="9"/>
+      <c r="BK9" s="9"/>
+      <c r="BL9" s="8"/>
+      <c r="BM9" s="8"/>
+      <c r="BN9" s="8"/>
+      <c r="BO9" s="8"/>
+      <c r="BP9" s="8"/>
+      <c r="BQ9" s="8"/>
+      <c r="BR9" s="8"/>
+      <c r="BS9" s="10"/>
+      <c r="BT9" s="10"/>
+      <c r="BU9" s="10"/>
+      <c r="BV9" s="10"/>
+    </row>
+    <row r="10" customHeight="1" spans="1:74">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="BC10" s="5"/>
+      <c r="BD10" s="5"/>
+      <c r="BE10" s="5"/>
+      <c r="BF10" s="5"/>
+      <c r="BG10" s="5"/>
+      <c r="BH10" s="5"/>
+      <c r="BI10" s="9"/>
+      <c r="BJ10" s="9"/>
+      <c r="BK10" s="9"/>
+      <c r="BL10" s="8"/>
+      <c r="BM10" s="8"/>
+      <c r="BN10" s="8"/>
+      <c r="BO10" s="8"/>
+      <c r="BP10" s="8"/>
+      <c r="BQ10" s="8"/>
+      <c r="BR10" s="8"/>
+      <c r="BS10" s="10"/>
+      <c r="BT10" s="10"/>
+      <c r="BU10" s="10"/>
+      <c r="BV10" s="10"/>
+    </row>
+    <row r="11" customHeight="1" spans="1:74">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="BC11" s="5"/>
+      <c r="BD11" s="5"/>
+      <c r="BE11" s="5"/>
+      <c r="BF11" s="5"/>
+      <c r="BG11" s="5"/>
+      <c r="BH11" s="5"/>
+      <c r="BI11" s="9"/>
+      <c r="BJ11" s="9"/>
+      <c r="BK11" s="9"/>
+      <c r="BL11" s="8"/>
+      <c r="BM11" s="8"/>
+      <c r="BN11" s="8"/>
+      <c r="BO11" s="8"/>
+      <c r="BP11" s="8"/>
+      <c r="BQ11" s="8"/>
+      <c r="BR11" s="8"/>
+      <c r="BS11" s="10"/>
+      <c r="BT11" s="10"/>
+      <c r="BU11" s="10"/>
+      <c r="BV11" s="10"/>
+    </row>
+    <row r="12" customHeight="1" spans="1:74">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="BC12" s="5"/>
+      <c r="BD12" s="5"/>
+      <c r="BE12" s="5"/>
+      <c r="BF12" s="5"/>
+      <c r="BG12" s="5"/>
+      <c r="BH12" s="5"/>
+      <c r="BI12" s="9"/>
+      <c r="BJ12" s="9"/>
+      <c r="BK12" s="9"/>
+      <c r="BL12" s="8"/>
+      <c r="BM12" s="8"/>
+      <c r="BN12" s="8"/>
+      <c r="BO12" s="8"/>
+      <c r="BP12" s="8"/>
+      <c r="BQ12" s="8"/>
+      <c r="BR12" s="8"/>
+      <c r="BS12" s="10"/>
+      <c r="BT12" s="10"/>
+      <c r="BU12" s="10"/>
+      <c r="BV12" s="10"/>
+    </row>
+    <row r="13" customHeight="1" spans="1:74">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="BC13" s="5"/>
+      <c r="BD13" s="5"/>
+      <c r="BE13" s="5"/>
+      <c r="BF13" s="5"/>
+      <c r="BG13" s="5"/>
+      <c r="BH13" s="5"/>
+      <c r="BI13" s="3"/>
+      <c r="BJ13" s="3"/>
+      <c r="BK13" s="3"/>
+      <c r="BL13" s="3"/>
+      <c r="BM13" s="3"/>
+      <c r="BN13" s="3"/>
+      <c r="BO13" s="3"/>
+      <c r="BP13" s="3"/>
+      <c r="BQ13" s="3"/>
+      <c r="BR13" s="3"/>
+      <c r="BS13" s="3"/>
+      <c r="BT13" s="3"/>
+      <c r="BU13" s="3"/>
+      <c r="BV13" s="3"/>
+    </row>
+    <row r="14" customHeight="1" spans="1:74">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14"/>
+      <c r="AN14"/>
+      <c r="AO14"/>
+      <c r="AP14"/>
+      <c r="AQ14"/>
+      <c r="AR14"/>
+      <c r="BC14" s="3"/>
+      <c r="BD14" s="3"/>
+      <c r="BE14" s="3"/>
+      <c r="BF14" s="3"/>
+      <c r="BG14" s="3"/>
+      <c r="BH14" s="3"/>
+      <c r="BI14" s="3"/>
+      <c r="BJ14" s="3"/>
+      <c r="BK14" s="3"/>
+      <c r="BL14" s="3"/>
+      <c r="BM14" s="3"/>
+      <c r="BN14" s="3"/>
+      <c r="BO14" s="3"/>
+      <c r="BP14" s="3"/>
+      <c r="BQ14" s="3"/>
+      <c r="BR14" s="3"/>
+      <c r="BS14" s="3"/>
+      <c r="BT14" s="3"/>
+      <c r="BU14" s="3"/>
+      <c r="BV14" s="3"/>
+    </row>
+    <row r="15" customHeight="1" spans="1:38">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+    </row>
+    <row r="16" customHeight="1" spans="1:38">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+    </row>
+    <row r="17" customHeight="1" spans="1:38">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+    </row>
+    <row r="18" customHeight="1" spans="1:38">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+    </row>
+    <row r="19" customHeight="1" spans="1:38">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="1"/>
+      <c r="AK19" s="1"/>
+      <c r="AL19" s="1"/>
+    </row>
+    <row r="20" customHeight="1" spans="1:38">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="1"/>
+      <c r="AK20" s="1"/>
+      <c r="AL20" s="1"/>
+    </row>
+    <row r="21" customHeight="1" spans="1:38">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="1"/>
+      <c r="AL21" s="1"/>
+    </row>
+    <row r="22" customHeight="1" spans="1:38">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="1"/>
+      <c r="AL22" s="1"/>
+    </row>
+    <row r="23" customHeight="1" spans="1:38">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+      <c r="AI23" s="1"/>
+      <c r="AJ23" s="1"/>
+      <c r="AK23" s="1"/>
+      <c r="AL23" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
@@ -964,7 +2247,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -981,7 +2264,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>